<commit_message>
changes added to test cases
</commit_message>
<xml_diff>
--- a/LanguageAndSkills_TestCases.xlsx
+++ b/LanguageAndSkills_TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umara\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IC TEST ANALYST\TAProgramme\MarsProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E838C-E60E-4A81-93B0-AA0A4D0E7E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F115A1B7-F406-4305-A18C-101A8E47C7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Skill not saved, page refreshed</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -981,6 +984,9 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
       <c r="E5" t="s">
         <v>39</v>
       </c>
@@ -1000,6 +1006,9 @@
       </c>
       <c r="C6" t="s">
         <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>148</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>

</xml_diff>